<commit_message>
Update Verification and validation plan.xlsx
</commit_message>
<xml_diff>
--- a/Project Management/Verification and validation plan.xlsx
+++ b/Project Management/Verification and validation plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\UNI\Year 3\GDIP\GDIP_ROBOT\Project Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Year 3\GDIP\Github\GDIP_ROBOT\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C3F21C-24DB-4BB1-A112-AF54B95E511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E49487-BB49-4ED6-9E38-AFA936A00974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verification and Validation Mat" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="100">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -114,9 +114,6 @@
     <t xml:space="preserve">Minimum Working Envolope </t>
   </si>
   <si>
-    <t>Saad &amp; John</t>
-  </si>
-  <si>
     <t>Pulling Arm out to 50cm</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>University</t>
   </si>
   <si>
-    <t>John &amp; Dominic</t>
-  </si>
-  <si>
     <t>3D printing redesigned parts</t>
   </si>
   <si>
@@ -153,18 +147,12 @@
     <t>James</t>
   </si>
   <si>
-    <t>James &amp; Emre</t>
-  </si>
-  <si>
     <t>Everyone agreed and signed off on all orders, documentation was kept</t>
   </si>
   <si>
     <t>Measures and moves resistor within 10 seconds</t>
   </si>
   <si>
-    <t>James &amp; Saad</t>
-  </si>
-  <si>
     <t>Lead team member's</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>Factor of saftey: 1</t>
   </si>
   <si>
-    <t>Emre &amp; Dom</t>
-  </si>
-  <si>
     <t>No parts broke due to stress or use</t>
   </si>
   <si>
@@ -207,9 +192,6 @@
     <t>Be ablt to lift 267mg</t>
   </si>
   <si>
-    <t>Dom &amp; James</t>
-  </si>
-  <si>
     <t>Electromagnet can hold more than one resistor at a time to well over the 267mg required</t>
   </si>
   <si>
@@ -249,9 +231,6 @@
     <t>Health and saftey documentation</t>
   </si>
   <si>
-    <t xml:space="preserve">Emre  </t>
-  </si>
-  <si>
     <t>Document reviewed by all and meets standards</t>
   </si>
   <si>
@@ -276,9 +255,6 @@
     <t>Code can run and be sent using bluetooth</t>
   </si>
   <si>
-    <t>James &amp; Dominic</t>
-  </si>
-  <si>
     <t>Possibility to run code in app</t>
   </si>
   <si>
@@ -304,6 +280,60 @@
   </si>
   <si>
     <t>UWE Fet Team</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Electronics and Programming lead</t>
+  </si>
+  <si>
+    <t>Algorithmic and Mathematical Lead</t>
+  </si>
+  <si>
+    <t>3D Design Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Administrator </t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>AML</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>EPL</t>
+  </si>
+  <si>
+    <t>3DD</t>
+  </si>
+  <si>
+    <t>AML &amp; 3DD</t>
+  </si>
+  <si>
+    <t>PM &amp; 3DD</t>
+  </si>
+  <si>
+    <t>EPL &amp; TA</t>
+  </si>
+  <si>
+    <t>EPL &amp; AML</t>
+  </si>
+  <si>
+    <t>TA &amp; PM</t>
+  </si>
+  <si>
+    <t>PM &amp; EPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA  </t>
+  </si>
+  <si>
+    <t>EPL &amp; PM</t>
   </si>
 </sst>
 </file>
@@ -491,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -545,7 +575,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +996,7 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="59.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -971,7 +1006,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -995,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>2</v>
@@ -1011,10 +1046,10 @@
         <v>3</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>5</v>
@@ -1059,7 +1094,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001</v>
@@ -1068,22 +1103,22 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>2.1</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="1" t="s">
@@ -1095,10 +1130,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="D5">
         <v>4.0999999999999996</v>
@@ -1107,7 +1142,7 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>1.2</v>
@@ -1116,13 +1151,13 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="1" t="s">
@@ -1134,10 +1169,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>4.2</v>
@@ -1146,13 +1181,13 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1160,10 +1195,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <v>3.1</v>
@@ -1172,7 +1207,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>1.3</v>
@@ -1181,16 +1216,16 @@
         <v>15</v>
       </c>
       <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
         <v>31</v>
       </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
@@ -1203,10 +1238,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D8">
         <v>3.2</v>
@@ -1215,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>1.1000000000000001</v>
@@ -1224,16 +1259,16 @@
         <v>15</v>
       </c>
       <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
         <v>31</v>
       </c>
-      <c r="J8" t="s">
-        <v>32</v>
-      </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
@@ -1246,10 +1281,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>4.3</v>
@@ -1258,13 +1293,13 @@
         <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1272,10 +1307,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D10">
         <v>4.4000000000000004</v>
@@ -1284,7 +1319,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>1.4</v>
@@ -1293,13 +1328,13 @@
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1307,10 +1342,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="D11">
         <v>1.5</v>
@@ -1319,13 +1354,13 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1333,10 +1368,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D12">
         <v>3.3</v>
@@ -1345,22 +1380,22 @@
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <v>2.2000000000000002</v>
       </c>
       <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
         <v>29</v>
       </c>
-      <c r="I12" t="s">
-        <v>30</v>
-      </c>
       <c r="J12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1368,10 +1403,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="D13">
         <v>4.5</v>
@@ -1380,13 +1415,13 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1394,10 +1429,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>4.2</v>
@@ -1406,13 +1441,13 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1420,19 +1455,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="D15">
         <v>2.2999999999999998</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15">
         <v>3.4</v>
@@ -1441,16 +1476,16 @@
         <v>17</v>
       </c>
       <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
         <v>31</v>
       </c>
-      <c r="J15" t="s">
-        <v>32</v>
-      </c>
       <c r="K15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
@@ -1463,10 +1498,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="D16">
         <v>3.5</v>
@@ -1475,13 +1510,13 @@
         <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1489,34 +1524,34 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>4.5999999999999996</v>
       </c>
       <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
         <v>29</v>
       </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>15</v>
-      </c>
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
       <c r="B19" s="7"/>
+      <c r="E19" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>87</v>
+      </c>
       <c r="J19" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
@@ -1525,97 +1560,106 @@
       <c r="O19" s="21"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
+      <c r="E20" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>18</v>
+      <c r="E21" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="O21" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>20</v>
+      <c r="E22" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>21</v>
-      </c>
       <c r="J24" s="17" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1681,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB9172-D8EC-4DC1-9900-127C73A49F4F}">
   <dimension ref="A2:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1761,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -1737,7 +1781,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -1757,7 +1801,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -1777,7 +1821,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -1794,7 +1838,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1805,7 +1849,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1816,7 +1860,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1827,7 +1871,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1838,10 +1882,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -1857,23 +1901,23 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1884,23 +1928,23 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1911,7 +1955,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1922,13 +1966,13 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1939,13 +1983,13 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1956,7 +2000,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1967,7 +2011,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1978,7 +2022,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1989,7 +2033,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2000,7 +2044,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>